<commit_message>
Applied presence Transhydrogenase for all organisms
</commit_message>
<xml_diff>
--- a/iFerment_assignments.xlsx
+++ b/iFerment_assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abeltingle/Documents/GitHub/iFerment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278A0BAB-2AAB-694B-A7F4-76489407CCC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3FABAF-BECE-614D-B045-851D0AF001C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="7100" windowWidth="18040" windowHeight="11880" xr2:uid="{3C0AD297-627C-BB48-99C2-62B05FC79ACD}"/>
+    <workbookView xWindow="10340" yWindow="3900" windowWidth="18040" windowHeight="11880" xr2:uid="{3C0AD297-627C-BB48-99C2-62B05FC79ACD}"/>
   </bookViews>
   <sheets>
     <sheet name="iFerment_assignments" sheetId="1" r:id="rId1"/>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB107D0F-33E2-D642-B950-A3F64C84BC6C}">
   <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="H238" sqref="H238"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -4927,11 +4927,11 @@
       <c r="F137" s="12">
         <v>1</v>
       </c>
-      <c r="G137" s="9">
-        <v>0</v>
-      </c>
-      <c r="H137" s="9">
-        <v>0</v>
+      <c r="G137" s="12">
+        <v>1</v>
+      </c>
+      <c r="H137" s="12">
+        <v>1</v>
       </c>
       <c r="I137" s="1"/>
     </row>

</xml_diff>